<commit_message>
Revisión Títulos Tema 3 Mat Grado 06
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion03/esqueletoGuion_MA_06_03_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion03/esqueletoGuion_MA_06_03_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EDITORIAL PLANETA\TEMA 3\SOLICITUDES GRAFICAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EDITORIAL PLANETA\TEMA 3\EDICION\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="83">
   <si>
     <t>FICHA</t>
   </si>
@@ -111,57 +111,24 @@
     <t>MT</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Adición de números naturales</t>
-  </si>
-  <si>
-    <t>La adición y sus propiedades</t>
-  </si>
-  <si>
-    <t>Adición y sustracción de números naturales</t>
-  </si>
-  <si>
-    <t>Sustracción de números naturales</t>
-  </si>
-  <si>
     <t>Practica la multiplicación de números naturales</t>
   </si>
   <si>
-    <t>Practica las propiedades de la multiplicación de números naturales</t>
-  </si>
-  <si>
-    <t>Competencias: Opera con números naturales y resuelve problemas</t>
-  </si>
-  <si>
     <t>MT_07_02</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: La sustracción de números naturales</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: La multiplicación de números naturales</t>
   </si>
   <si>
     <t>Ejercita la división de números naturales</t>
   </si>
   <si>
-    <t>Situaciones problema con multiplicación y división</t>
-  </si>
-  <si>
     <t>La división de números naturales</t>
   </si>
   <si>
     <t>Las operaciones combinadas con números naturales</t>
   </si>
   <si>
-    <t>Las operaciones combinadas</t>
-  </si>
-  <si>
-    <t>Operaciones combinadas en situaciones problema</t>
-  </si>
-  <si>
-    <t>Operaciones combinadas con números naturales</t>
-  </si>
-  <si>
     <t>Propiedades de la adición</t>
   </si>
   <si>
@@ -213,9 +180,6 @@
     <t>si</t>
   </si>
   <si>
-    <t>Lo que debes recordar de las operaciones con números naturales</t>
-  </si>
-  <si>
     <t>La adición de números naturales</t>
   </si>
   <si>
@@ -274,6 +238,48 @@
   </si>
   <si>
     <t>Webs de referencia</t>
+  </si>
+  <si>
+    <t>Practica la suma de números naturales</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La suma de números naturales</t>
+  </si>
+  <si>
+    <t>La suma y la resta de números naturales</t>
+  </si>
+  <si>
+    <t>Ejercita la resta de números naturales</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La resta de números naturales</t>
+  </si>
+  <si>
+    <t>Practica las propiedades de la suma y la multiplicación</t>
+  </si>
+  <si>
+    <t>Opera con multiplicaciones y divisiones</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La división de números naturales</t>
+  </si>
+  <si>
+    <t>Practica las operaciones combinadas con números naturales</t>
+  </si>
+  <si>
+    <t>¿Cuáles son los pasos para resolver el problema?</t>
+  </si>
+  <si>
+    <t>Soluciona problemas de aplicación con operaciones combinadas</t>
+  </si>
+  <si>
+    <t>Lo que debes recordar sobre operaciones con números naturales</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Las operaciones combinadas de naturales</t>
+  </si>
+  <si>
+    <t>Competencias: opera con números naturales y resuelve problemas</t>
   </si>
 </sst>
 </file>
@@ -1593,7 +1599,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1639,10 +1645,10 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1665,10 +1671,10 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" t="s">
         <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -1685,10 +1691,10 @@
         <v>19</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -1705,10 +1711,10 @@
         <v>19</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F5">
         <v>6</v>
@@ -1725,10 +1731,10 @@
         <v>19</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F6">
         <v>9</v>
@@ -1745,10 +1751,10 @@
         <v>19</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F7">
         <v>12</v>
@@ -1765,10 +1771,10 @@
         <v>19</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F8">
         <v>14</v>
@@ -1785,10 +1791,10 @@
         <v>19</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F9">
         <v>15</v>
@@ -1806,10 +1812,10 @@
         <v>19</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F10">
         <v>16</v>
@@ -1827,10 +1833,10 @@
         <v>19</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F11">
         <v>17</v>
@@ -1848,10 +1854,10 @@
         <v>19</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F12">
         <v>18</v>
@@ -1869,10 +1875,10 @@
         <v>19</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F13">
         <v>19</v>
@@ -1889,10 +1895,10 @@
         <v>19</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F14">
         <v>20</v>
@@ -1909,10 +1915,10 @@
         <v>19</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F15">
         <v>21</v>
@@ -1929,10 +1935,10 @@
         <v>19</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F16">
         <v>22</v>
@@ -1949,10 +1955,10 @@
         <v>19</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F17">
         <v>23</v>
@@ -1969,10 +1975,10 @@
         <v>19</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F18">
         <v>24</v>
@@ -1989,10 +1995,10 @@
         <v>19</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="E19" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F19">
         <v>31</v>
@@ -2039,10 +2045,10 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -2050,10 +2056,10 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -2061,10 +2067,10 @@
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C4">
         <v>7</v>
@@ -2072,10 +2078,10 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C5">
         <v>8</v>
@@ -2083,10 +2089,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -2094,10 +2100,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <v>11</v>
@@ -2105,10 +2111,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C8">
         <v>13</v>
@@ -2116,10 +2122,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>25</v>
@@ -2127,10 +2133,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C10">
         <v>26</v>
@@ -2138,10 +2144,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C11">
         <v>27</v>
@@ -2149,10 +2155,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C12">
         <v>28</v>
@@ -2160,10 +2166,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C13">
         <v>29</v>
@@ -2171,10 +2177,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C14">
         <v>30</v>
@@ -2182,10 +2188,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C15">
         <v>32</v>
@@ -2193,10 +2199,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C16">
         <v>33</v>
@@ -2223,8 +2229,8 @@
   </sheetPr>
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,10 +2256,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2261,10 +2267,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2272,10 +2278,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2283,10 +2289,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2294,10 +2300,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2305,10 +2311,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2316,10 +2322,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2327,10 +2333,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2338,10 +2344,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2349,10 +2355,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2360,10 +2366,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2371,10 +2377,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2382,10 +2388,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2393,10 +2399,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2404,10 +2410,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2415,10 +2421,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2426,10 +2432,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2437,10 +2443,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2448,10 +2454,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2459,10 +2465,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2470,10 +2476,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2481,10 +2487,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2492,10 +2498,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2503,10 +2509,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2514,10 +2520,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2525,10 +2531,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2536,10 +2542,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2547,10 +2553,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2558,10 +2564,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2569,10 +2575,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2580,10 +2586,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2591,10 +2597,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2602,10 +2608,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2625,10 +2631,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="E56" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2642,7 +2648,7 @@
     <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -2671,15 +2677,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -2687,15 +2693,15 @@
       <c r="G2" s="9"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2703,15 +2709,15 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -2719,143 +2725,155 @@
       <c r="G4" s="9"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="9" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="9" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="5" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="9" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="5" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="9" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="9" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="5" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="J9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="9" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -2863,15 +2881,15 @@
       <c r="G11" s="9"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -2879,15 +2897,15 @@
       <c r="G12" s="9"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -2895,189 +2913,207 @@
       <c r="G13" s="9"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="9" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="9" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="5" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="J15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="9" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="5" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="J16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="9" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J17">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="9" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="5" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="9" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="5" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="J20">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="9" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="5" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -3085,15 +3121,15 @@
       <c r="G22" s="9"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -3101,15 +3137,15 @@
       <c r="G23" s="9"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -3117,15 +3153,15 @@
       <c r="G24" s="9"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -3133,777 +3169,843 @@
       <c r="G25" s="9"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C26" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H27" t="s">
+        <v>38</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H28" t="s">
+        <v>26</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J28">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" t="s">
+        <v>39</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H31" t="s">
+        <v>74</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J31">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" t="s">
+        <v>28</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J33">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H43" t="s">
+        <v>29</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J43">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H45" t="s">
+        <v>75</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J45">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H47" t="s">
+        <v>76</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J47">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H51" t="s">
+        <v>77</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J51">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H52" t="s">
+        <v>78</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J52">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="8" t="s">
+      <c r="H53" t="s">
+        <v>31</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J53">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H54" t="s">
+        <v>79</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J54">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H55" t="s">
+        <v>80</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J55">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H57" t="s">
+        <v>81</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J57">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H60" t="s">
+        <v>40</v>
+      </c>
+      <c r="I60" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J60">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H62" t="s">
+        <v>41</v>
+      </c>
+      <c r="I62" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J62">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H63" t="s">
+        <v>42</v>
+      </c>
+      <c r="I63" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J63">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H27" t="s">
-        <v>49</v>
-      </c>
-      <c r="I27" s="5" t="s">
+      <c r="E64" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H69" t="s">
+        <v>43</v>
+      </c>
+      <c r="I69" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J69">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H70" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H28" t="s">
-        <v>30</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="I70" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J70">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H31" t="s">
-        <v>31</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H33" t="s">
-        <v>35</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H43" t="s">
-        <v>36</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H45" t="s">
-        <v>37</v>
-      </c>
-      <c r="I45" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H47" t="s">
-        <v>38</v>
-      </c>
-      <c r="I47" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>19</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>19</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H51" t="s">
-        <v>39</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>19</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H52" t="s">
-        <v>40</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>19</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H53" t="s">
-        <v>39</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>19</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H54" t="s">
-        <v>41</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H55" t="s">
-        <v>60</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H57" t="s">
-        <v>42</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>19</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H60" t="s">
-        <v>51</v>
-      </c>
-      <c r="I60" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>19</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>19</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H62" t="s">
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E72" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I62" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>19</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H63" t="s">
-        <v>53</v>
-      </c>
-      <c r="I63" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>19</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>19</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>19</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>19</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>19</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>19</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I69" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>19</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H70" t="s">
-        <v>55</v>
-      </c>
-      <c r="I70" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>19</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>19</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="H72" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I72" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J72">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>19</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>19</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="H74" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="I74" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="J74">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>19</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>19</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="H76" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J76">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>19</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edición Tema 3 Mat 06
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion03/esqueletoGuion_MA_06_03_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion03/esqueletoGuion_MA_06_03_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EDITORIAL PLANETA\TEMA 3\EDICION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EDITORIAL PLANETA\TEMA 3\EDICION 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="81">
   <si>
     <t>FICHA</t>
   </si>
@@ -96,18 +96,12 @@
     <t>MA_06_03_CO</t>
   </si>
   <si>
-    <t>En nuestra vida diaria se presentan situaciones en las que es necesario el uso de operaciones aritméticas para dar solución a ellas; atrévete a conocerlas!!!</t>
-  </si>
-  <si>
     <t>Educación Básica Secundaria</t>
   </si>
   <si>
     <t>Matemáticas</t>
   </si>
   <si>
-    <t xml:space="preserve">6° </t>
-  </si>
-  <si>
     <t>MT</t>
   </si>
   <si>
@@ -168,9 +162,6 @@
     <t>Solución de inecuaciones</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: La solución de las inecuaciones</t>
-  </si>
-  <si>
     <t>Mapa conceptual</t>
   </si>
   <si>
@@ -201,15 +192,9 @@
     <t>¿Qué propiedades cumple la sustracción de números naturales?</t>
   </si>
   <si>
-    <t>Profundiza</t>
-  </si>
-  <si>
     <t>La multiplicación de números naturales</t>
   </si>
   <si>
-    <t>Foto</t>
-  </si>
-  <si>
     <t>Las propiedades de la multiplicación de números naturales</t>
   </si>
   <si>
@@ -252,9 +237,6 @@
     <t>Ejercita la resta de números naturales</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: La resta de números naturales</t>
-  </si>
-  <si>
     <t>Practica las propiedades de la suma y la multiplicación</t>
   </si>
   <si>
@@ -280,6 +262,18 @@
   </si>
   <si>
     <t>Competencias: opera con números naturales y resuelve problemas</t>
+  </si>
+  <si>
+    <t>En nuestra vida diaria se presentan situaciones en las que es necesario el uso de operaciones aritméticas: pagar un servicio, recibir un beneficio, repartir gastos, multiplicar ganancias y muchas más. Recuerda las operaciones y propiedades de los números naturales para dar solución a estas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1°  </t>
+  </si>
+  <si>
+    <t>Propiedades de la Sustracción</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: la solución de las inecuaciones</t>
   </si>
 </sst>
 </file>
@@ -806,7 +800,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -843,6 +837,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1523,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,38 +1552,53 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="19"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:B6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1596,10 +1611,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,22 +1651,22 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2"/>
       <c r="H2"/>
@@ -1662,350 +1677,330 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
       <c r="F3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
       <c r="F4">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
       <c r="F5">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
       <c r="F6">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
       <c r="F7">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
       <c r="F8">
-        <v>14</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
       <c r="F9">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
       <c r="F10">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
-      </c>
       <c r="F11">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" t="s">
-        <v>27</v>
-      </c>
       <c r="F12">
-        <v>18</v>
-      </c>
-      <c r="G12" s="10"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
-      </c>
       <c r="F13">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" t="s">
-        <v>27</v>
-      </c>
       <c r="F14">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15">
         <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15">
-        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" t="s">
         <v>25</v>
       </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" t="s">
-        <v>27</v>
-      </c>
       <c r="F16">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" t="s">
         <v>25</v>
       </c>
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" t="s">
-        <v>27</v>
-      </c>
       <c r="F17">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" t="s">
         <v>25</v>
       </c>
-      <c r="C18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" t="s">
-        <v>27</v>
-      </c>
       <c r="F18">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="16"/>
+      <c r="D19" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2020,10 +2015,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,167 +2040,200 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C8">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16">
-        <v>33</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2227,10 +2255,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,10 +2284,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2267,10 +2295,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2278,10 +2306,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2289,10 +2317,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2300,10 +2328,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2311,10 +2339,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2322,10 +2350,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2333,10 +2361,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2344,10 +2372,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2355,10 +2383,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2366,10 +2394,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2377,10 +2405,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2388,10 +2416,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2399,10 +2427,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2410,10 +2438,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2421,10 +2449,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2432,10 +2460,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2443,10 +2471,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2454,10 +2482,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2465,10 +2493,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2476,10 +2504,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2487,10 +2515,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2498,10 +2526,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2509,10 +2537,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2520,10 +2548,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2531,10 +2559,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2542,10 +2570,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2553,10 +2581,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2564,10 +2592,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2575,10 +2603,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2586,10 +2614,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2597,10 +2625,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2608,10 +2636,32 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>33</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2631,11 +2681,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E56" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2644,11 +2692,11 @@
     <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
     <col min="5" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.140625" customWidth="1"/>
+    <col min="8" max="8" width="68.28515625" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -2677,15 +2725,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -2693,15 +2741,15 @@
       <c r="G2" s="9"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2709,15 +2757,15 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -2725,187 +2773,186 @@
       <c r="G4" s="9"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H6" s="5"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="9" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="9" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="5" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J9">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H10" s="5"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+        <v>46</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -2913,1099 +2960,1078 @@
       <c r="G13" s="9"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>50</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>56</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
-      <c r="H15" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J15">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
-      <c r="H16" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J16">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H16" s="5"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H17" s="5"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J19">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J20">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J21">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+      <c r="E22" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
+      <c r="E24" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
+        <v>51</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H32" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H34" t="s">
+        <v>37</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H35" t="s">
+        <v>68</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H37" t="s">
+        <v>26</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H46" t="s">
+        <v>27</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I47" s="9"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H48" t="s">
+        <v>69</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I49" s="9"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H50" t="s">
+        <v>70</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H54" t="s">
+        <v>71</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H55" t="s">
+        <v>72</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="H56" t="s">
+        <v>29</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H57" t="s">
+        <v>73</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H58" t="s">
+        <v>74</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="E59" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H60" t="s">
+        <v>76</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I27" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J27">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H28" t="s">
-        <v>26</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J28">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="E62" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I62" s="9"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H63" t="s">
+        <v>38</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I64" s="9"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H65" t="s">
+        <v>39</v>
+      </c>
+      <c r="I65" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H66" t="s">
+        <v>40</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E67" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I71" s="9"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H72" t="s">
+        <v>41</v>
+      </c>
+      <c r="I72" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H73" t="s">
+        <v>42</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H30" t="s">
-        <v>39</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J30">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H31" t="s">
-        <v>74</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J31">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="E74" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I74" s="9"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>19</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H33" t="s">
-        <v>28</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J33">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H43" t="s">
-        <v>29</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J43">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H45" t="s">
-        <v>75</v>
-      </c>
-      <c r="I45" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J45">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H47" t="s">
-        <v>76</v>
-      </c>
-      <c r="I47" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J47">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48" s="8" t="s">
+      <c r="E75" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H75" t="s">
+        <v>80</v>
+      </c>
+      <c r="I75" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>19</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>19</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H51" t="s">
-        <v>77</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J51">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>19</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H52" t="s">
-        <v>78</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J52">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>19</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H53" t="s">
-        <v>31</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J53">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>19</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H54" t="s">
-        <v>79</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J54">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H55" t="s">
-        <v>80</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J55">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H57" t="s">
-        <v>81</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J57">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>19</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H60" t="s">
-        <v>40</v>
-      </c>
-      <c r="I60" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J60">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>19</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>19</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H62" t="s">
-        <v>41</v>
-      </c>
-      <c r="I62" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J62">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>19</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H63" t="s">
-        <v>42</v>
-      </c>
-      <c r="I63" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J63">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>19</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>19</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>19</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>19</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>19</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>19</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H69" t="s">
-        <v>43</v>
-      </c>
-      <c r="I69" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J69">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>19</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H70" t="s">
-        <v>44</v>
-      </c>
-      <c r="I70" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J70">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>19</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>19</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H72" t="s">
-        <v>45</v>
-      </c>
-      <c r="I72" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J72">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>19</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>19</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H74" t="s">
-        <v>82</v>
-      </c>
-      <c r="I74" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J74">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>19</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>19</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H76" t="s">
-        <v>47</v>
-      </c>
-      <c r="I76" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J76">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I76" s="9"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>19</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>68</v>
+        <v>49</v>
+      </c>
+      <c r="H77" t="s">
+        <v>76</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>19</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>19</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>